<commit_message>
Update files for 7
</commit_message>
<xml_diff>
--- a/prosym07_1966/7.xlsx
+++ b/prosym07_1966/7.xlsx
@@ -139,7 +139,7 @@
     <t>WPRO1966toc.pdf</t>
   </si>
   <si>
-    <t>セッションA</t>
+    <t>A</t>
   </si>
   <si>
     <t>WPRO1966A00.pdf</t>
@@ -271,7 +271,7 @@
     <t>A-76</t>
   </si>
   <si>
-    <t>セッションB</t>
+    <t>B</t>
   </si>
   <si>
     <t>WPRO1966B00.pdf</t>
@@ -382,7 +382,7 @@
     <t>B-56</t>
   </si>
   <si>
-    <t>セッションC</t>
+    <t>C</t>
   </si>
   <si>
     <t>WPRO1966C00.pdf</t>
@@ -514,7 +514,7 @@
     <t>C-114</t>
   </si>
   <si>
-    <t>セッションD</t>
+    <t>D</t>
   </si>
   <si>
     <t>WPRO1966D00.pdf</t>
@@ -622,7 +622,7 @@
     <t>D-53</t>
   </si>
   <si>
-    <t>セッション自由討論</t>
+    <t>自由討論</t>
   </si>
   <si>
     <t>WPRO1966F00.pdf</t>

</xml_diff>